<commit_message>
adds to ticker xlsx and fixes financial times bug in summary.py
</commit_message>
<xml_diff>
--- a/backend/ticker.xlsx
+++ b/backend/ticker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilycroxall/Documents/sentiment-analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilycroxall/Documents/sentiment-analysis/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73C1D73-97F5-F046-B329-77F8B2889DBC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBD24D9-AC76-E646-8D34-CA8E834C327B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2140" yWindow="460" windowWidth="24400" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="676">
   <si>
     <t>Name</t>
   </si>
@@ -2047,6 +2047,12 @@
   </si>
   <si>
     <t>Tesla, Inc.</t>
+  </si>
+  <si>
+    <t>BNP Paribas</t>
+  </si>
+  <si>
+    <t>BNPQF</t>
   </si>
 </sst>
 </file>
@@ -2398,10 +2404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B339"/>
+  <dimension ref="A1:B340"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A309" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B340" sqref="B340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5122,6 +5128,14 @@
         <v>672</v>
       </c>
     </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A340" t="s">
+        <v>674</v>
+      </c>
+      <c r="B340" t="s">
+        <v>675</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>